<commit_message>
simple example by modules
</commit_message>
<xml_diff>
--- a/rest-get/src/test/resources/rest/rest-get.xlsx
+++ b/rest-get/src/test/resources/rest/rest-get.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\december-release\microservices-lowcode-testautomation\rest-get\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D2FA20-2204-4896-8F29-F4FA64904559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9CBC69-1C3F-4FC1-B39A-B60567B98B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>EvaluateFunctionVariables</t>
-  </si>
-  <si>
-    <t>ReadCustomers-Simple</t>
   </si>
   <si>
     <t>dateOfBirth,firstName,lastName,lastTimeOnline,spokenLanguages/additionalProp1:additionalProp2:additionalProp3,username
@@ -100,13 +97,28 @@
     <t>@examples</t>
   </si>
   <si>
-    <t>Read Customer infos - Example</t>
-  </si>
-  <si>
     <t>https://localhost/persons/bgates</t>
   </si>
   <si>
     <t>ep</t>
+  </si>
+  <si>
+    <t>ReadPerson-Simple</t>
+  </si>
+  <si>
+    <t>Read user infos - Example</t>
+  </si>
+  <si>
+    <t>ReadPetByQueryparams-Simple</t>
+  </si>
+  <si>
+    <t>Read pet by customer by query params</t>
+  </si>
+  <si>
+    <t>status=available</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/pets/findByTags?tags=red</t>
   </si>
 </sst>
 </file>
@@ -263,7 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -282,6 +294,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -597,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +621,7 @@
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -648,7 +661,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>11</v>
@@ -663,24 +676,24 @@
         <v>15</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
@@ -695,15 +708,45 @@
       <c r="J2" s="12"/>
       <c r="K2" s="10"/>
       <c r="L2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6">
+        <v>200</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{4201C29B-B67D-48C2-92AE-011AA2CEB9F2}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{7059204A-A98F-4B4D-A8DC-1C624ACC96C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Allure report configuration
</commit_message>
<xml_diff>
--- a/rest-get/src/test/resources/rest/rest-get.xlsx
+++ b/rest-get/src/test/resources/rest/rest-get.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\december-release\microservices-lowcode-testautomation\rest-get\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9CBC69-1C3F-4FC1-B39A-B60567B98B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8D50D-1BAB-45B3-853E-64B85B88573A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -118,7 +118,7 @@
     <t>status=available</t>
   </si>
   <si>
-    <t>https://live.virtualandemo.com/pets/findByTags?tags=red</t>
+    <t>https://localhost/pets/findByTags?tags=red</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated with JSON schema validation
</commit_message>
<xml_diff>
--- a/rest-get/src/test/resources/rest/rest-get.xlsx
+++ b/rest-get/src/test/resources/rest/rest-get.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-get\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA3AE2D-9CBC-4A00-B951-3F26ED5944C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D396BFF-1B10-448E-9A39-C966C26F3090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -110,13 +110,23 @@
   </si>
   <si>
     <t xml:space="preserve"> @simple-get  @complete-response-validation</t>
+  </si>
+  <si>
+    <t>id,name,status
+i~201,,available</t>
+  </si>
+  <si>
+    <t>SchemaValidation</t>
+  </si>
+  <si>
+    <t>pets_json.schema.json=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,26 +135,42 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Amasis MT Pro Medium"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF2C3E50"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
+      <name val="Amasis MT Pro Medium"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Amasis MT Pro Medium"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Amasis MT Pro Medium"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -185,26 +211,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{EC4A6B07-6E56-4BDE-8E7E-6360AB6100FA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -516,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,16 +558,16 @@
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="65.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,13 +596,16 @@
         <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -597,14 +631,15 @@
         <v>200</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -632,8 +667,13 @@
       <c r="I3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -643,5 +683,6 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{7059204A-A98F-4B4D-A8DC-1C624ACC96C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with 1.6.4 release
</commit_message>
<xml_diff>
--- a/rest-get/src/test/resources/rest/rest-get.xlsx
+++ b/rest-get/src/test/resources/rest/rest-get.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-get\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D396BFF-1B10-448E-9A39-C966C26F3090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A93C1-F821-4E28-8FA6-CC388B4302C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>SchemaValidation</t>
   </si>
   <si>
-    <t>pets_json.schema.json=true</t>
+    <t>pets_json.schema.json=false</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated with JSONSchema message type example
</commit_message>
<xml_diff>
--- a/rest-get/src/test/resources/rest/rest-get.xlsx
+++ b/rest-get/src/test/resources/rest/rest-get.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-get\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EEF80C-702D-411F-B336-AD6E1A10D1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D911B8B-7C2A-46DB-9E82-BADA3581B345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="39" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -639,7 +639,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="39" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>